<commit_message>
Add Receipt maker feature
</commit_message>
<xml_diff>
--- a/receipt_recorder_arar_maker_v2/ARAR.xlsx
+++ b/receipt_recorder_arar_maker_v2/ARAR.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -51,7 +50,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,28 +485,20 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>juanito</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>43</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Invoice Total</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>12345</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>45076</v>
-      </c>
-      <c r="E2" t="n">
-        <v>12</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n"/>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>12345</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -519,35 +510,6 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Invoice Total</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>12345</v>
-      </c>
-      <c r="D3" s="1" t="n"/>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>12345</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>